<commit_message>
Created the .py file for this project
. py (Loans.py) created for code testing
README.txt created for logging info

First pass data cleaning
</commit_message>
<xml_diff>
--- a/udacity final report/Prosper Loan Data - Variable Definitions.xlsx
+++ b/udacity final report/Prosper Loan Data - Variable Definitions.xlsx
@@ -1,12 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -508,73 +511,485 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49:A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="36.14"/>
-    <col customWidth="1" min="2" max="2" width="108.29"/>
-    <col customWidth="1" min="3" max="20" width="17.29"/>
+    <col min="1" max="1" width="36.140625" customWidth="1"/>
+    <col min="2" max="2" width="204.28515625" customWidth="1"/>
+    <col min="3" max="20" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,39 +997,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -622,7 +1037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -630,7 +1045,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -638,671 +1053,671 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
         <v>60</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
         <v>62</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
         <v>76</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="12" t="s">
         <v>78</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="12" t="s">
         <v>80</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
         <v>82</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
         <v>86</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
         <v>90</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
         <v>92</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="15" t="s">
         <v>94</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="13" t="s">
         <v>96</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="13" t="s">
         <v>98</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="13" t="s">
         <v>100</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
         <v>102</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
         <v>104</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
         <v>108</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="15" t="s">
         <v>110</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="15" t="s">
         <v>112</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="15" t="s">
         <v>120</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="15" t="s">
         <v>122</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="15" t="s">
         <v>124</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="15" t="s">
         <v>126</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="15" t="s">
         <v>128</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="15" t="s">
         <v>130</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="15" t="s">
         <v>132</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
         <v>142</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
         <v>148</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
         <v>150</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
         <v>152</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
         <v>154</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
         <v>156</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
         <v>158</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
         <v>160</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="83" ht="14.25" customHeight="1">
+    <row r="83" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
-    </row>
-    <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
-    </row>
-    <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
-    </row>
-    <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="3"/>
-      <c r="B90" s="3"/>
-    </row>
-    <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="3"/>
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="3"/>
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" s="3"/>
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
-    </row>
-    <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="3"/>
-      <c r="B95" s="3"/>
-    </row>
-    <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="3"/>
-      <c r="B96" s="3"/>
-    </row>
-    <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="3"/>
-      <c r="B97" s="3"/>
-    </row>
-    <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="3"/>
-      <c r="B98" s="3"/>
-    </row>
-    <row r="99" ht="14.25" customHeight="1">
-      <c r="A99" s="3"/>
-      <c r="B99" s="3"/>
-    </row>
-    <row r="100" ht="14.25" customHeight="1">
-      <c r="A100" s="3"/>
-      <c r="B100" s="3"/>
+      <c r="B83" s="2"/>
+    </row>
+    <row r="84" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
+    </row>
+    <row r="86" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="2"/>
+      <c r="B86" s="2"/>
+    </row>
+    <row r="87" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+    </row>
+    <row r="88" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2"/>
+    </row>
+    <row r="89" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2"/>
+    </row>
+    <row r="90" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="2"/>
+      <c r="B90" s="2"/>
+    </row>
+    <row r="91" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
+    </row>
+    <row r="92" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2"/>
+    </row>
+    <row r="93" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2"/>
+    </row>
+    <row r="94" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="2"/>
+      <c r="B94" s="2"/>
+    </row>
+    <row r="95" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+    </row>
+    <row r="96" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="2"/>
+      <c r="B96" s="2"/>
+    </row>
+    <row r="97" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="2"/>
+      <c r="B97" s="2"/>
+    </row>
+    <row r="98" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="2"/>
+      <c r="B98" s="2"/>
+    </row>
+    <row r="99" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="2"/>
+      <c r="B99" s="2"/>
+    </row>
+    <row r="100" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>